<commit_message>
Do some sentence embedding with AR50 and matrikkel documentation
</commit_message>
<xml_diff>
--- a/documents/Q&As.xlsx
+++ b/documents/Q&As.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ABB69C-6349-4CF9-8D0D-12C62A5B40A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC37E145-E80B-49AC-9162-7BC61FA9B734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -76,15 +76,52 @@
   <si>
     <t>Dataset containing building points: "\\wsl.localhost\Ubuntu\home\dev\master-thesis\data\bygninger_100årsflom.shp"</t>
   </si>
+  <si>
+    <t>How many percent of buildings have more than 2km to the nearest "Videregående skole"?</t>
+  </si>
+  <si>
+    <t>~31%</t>
+  </si>
+  <si>
+    <t>Steps:
+1) Gather and load building point  data and its documentation
+2) Find the "bygningstype" field and check the documentation to see that "Videregående skole" has type 616
+3) Select building points that have "bygninigstype" = 616
+4) Create a 2-kilometer buffer around the selected points
+5) Optionally dissolve the buffers
+6) Perform an difference or intersection operation to separate points that are inside/outside the buffer(s)
+7) Perform the percentage calculations</t>
+  </si>
+  <si>
+    <t>53,855283 km^2</t>
+  </si>
+  <si>
+    <t>Determine how many square kilometers have high forest productivity.</t>
+  </si>
+  <si>
+    <t>Steps:
+1) Gather and load building point AR50 data , either the entire series or only "Jordbruk", along with the AR50 documentation
+2) Find the "skogbonitet" field and check the documentation to see that areas with the highest forest productivity have value 18.
+3) Select building points that have "skogbonitet" = 18
+4) Calculate the area of each selected polygon.
+5) Sum all areas.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -192,6 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,6 +567,28 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add friluft to QGIS
</commit_message>
<xml_diff>
--- a/documents/Q&As.xlsx
+++ b/documents/Q&As.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC37E145-E80B-49AC-9162-7BC61FA9B734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5D4FDD-753C-4550-9B08-88A3906C5757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -99,19 +99,62 @@
     <t>Determine how many square kilometers have high forest productivity.</t>
   </si>
   <si>
+    <t xml:space="preserve">Is the area predominantly coniferous or deciduous forest? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is about 250km^2 coniferous forest and 17km^2 deciduous forest. Thus, the area is predominantly coniferous. </t>
+  </si>
+  <si>
     <t>Steps:
 1) Gather and load building point AR50 data , either the entire series or only "Jordbruk", along with the AR50 documentation
-2) Find the "skogbonitet" field and check the documentation to see that areas with the highest forest productivity have value 18.
+2) Find the "skogbonitet" field and check the documentation to see that areas with the highest forest productivity have value 18
+3) Select building points that have "skogbonitet" = 18
+4) Calculate the area of each selected polygon
+5) Sum all areas</t>
+  </si>
+  <si>
+    <t>Steps:
+1) Gather and load building point AR50 data , either the entire series or only "Jordbruk", along with the AR50 documentation
+2) Find the "skogbonitet" field and check the documentation to see that areas with the highest forest productivity have value 18
 3) Select building points that have "skogbonitet" = 18
 4) Calculate the area of each selected polygon.
-5) Sum all areas.</t>
+5) Sum all areas</t>
+  </si>
+  <si>
+    <t>Are there any cultural heritage sites within this bounding box?
+[
+    [63.4159261840723, 10.449447170396198],
+    [63.42364892527119, 10.449837255689479],
+    [63.42345265401785, 10.46906466674888],
+    [63.4157299786334, 10.46866941273723],
+    [63.4159261840723, 10.449447170396198] 
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are three cultural heritage sites within the bounding box. </t>
+  </si>
+  <si>
+    <t>Steps:
+1) Gather and load building point cultural heritage point data
+2) Create a bounding box polygon
+3) Do "is-point-within" analysis, filtering the cultural heritage data
+4) Count the number of rows after filtering</t>
+  </si>
+  <si>
+    <t>How many schools buildings are there?</t>
+  </si>
+  <si>
+    <t>Steps:
+1) Gather and load building point  data and its documentation
+2) Find all "bygningstype" values that correspond to some type of school building
+3) Count the rows after filtering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +165,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -230,6 +279,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,26 +617,57 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add analysis Excel table
</commit_message>
<xml_diff>
--- a/documents/Q&As.xlsx
+++ b/documents/Q&As.xlsx
@@ -8,46 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5D4FDD-753C-4550-9B08-88A3906C5757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD725F1F-0B61-4FEF-B3FA-22B02044666F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t xml:space="preserve">Question </t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>Reasoning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me all Norwegian municipalities with population greater than 100 000. </t>
-  </si>
-  <si>
-    <t>Steps: 
-1) Load dataset x
-2) Find the relevnat attribute ("innbyggertall")
-3) Create a filter operation ("innbyggertall &gt; 100 000")
-4) Use filter operation to create subset of dataset x</t>
-  </si>
-  <si>
-    <t>Table containing Oslo, Bergen, Trondheim, Stavanger, Bærum, Kristiansand, and Drammen</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Find all buildings that are in the danger zone of a being flooded, in accordnace to current regulations for new buildings. </t>
   </si>
@@ -141,13 +130,47 @@
 4) Count the number of rows after filtering</t>
   </si>
   <si>
-    <t>How many schools buildings are there?</t>
+    <t>flood_buildings</t>
+  </si>
+  <si>
+    <t>noisy_roads</t>
+  </si>
+  <si>
+    <t>school_count</t>
+  </si>
+  <si>
+    <t>vgs_vicinity</t>
+  </si>
+  <si>
+    <t>forest_types</t>
+  </si>
+  <si>
+    <t>cultural_heritage_bbox</t>
+  </si>
+  <si>
+    <t>analysis_id</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>reasoning</t>
+  </si>
+  <si>
+    <t>How many hotels are there?</t>
   </si>
   <si>
     <t>Steps:
 1) Gather and load building point  data and its documentation
-2) Find all "bygningstype" values that correspond to some type of school building
+2) Find all "bygningstype" values that correspond a hotel ("Hotellbygning" --&gt; 551)
 3) Count the rows after filtering</t>
+  </si>
+  <si>
+    <t>Number of hotels: 28
+Dataset: "\\wsl.localhost\Ubuntu\home\dev\master-thesis\data\hotels.shp"</t>
   </si>
 </sst>
 </file>
@@ -176,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,39 +212,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -231,55 +228,30 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,114 +532,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="49.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="D8" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Postgres DB and OGC API Features services, and perform simple CQL test
</commit_message>
<xml_diff>
--- a/documents/Q&As.xlsx
+++ b/documents/Q&As.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD725F1F-0B61-4FEF-B3FA-22B02044666F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8267D-DB3B-4F00-A3DE-C961B96B9C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="-15" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">Find all buildings that are in the danger zone of a being flooded, in accordnace to current regulations for new buildings. </t>
   </si>
@@ -171,6 +171,19 @@
   <si>
     <t>Number of hotels: 28
 Dataset: "\\wsl.localhost\Ubuntu\home\dev\master-thesis\data\hotels.shp"</t>
+  </si>
+  <si>
+    <t>Postal code</t>
+  </si>
+  <si>
+    <t>Get the postal code of Sorgenfrivegen 12B.</t>
+  </si>
+  <si>
+    <t>Steps: 
+1) Gather and load address point data 
+2) Find the "adresseTekst" attribute 
+3) Find the closest matching address, if any
+4) Get the entire row, and look up the "postnummer" attribute</t>
   </si>
 </sst>
 </file>
@@ -240,14 +253,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -532,127 +544,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="43.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7031</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before LangGraph SQL worker
</commit_message>
<xml_diff>
--- a/documents/Q&As.xlsx
+++ b/documents/Q&As.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8267D-DB3B-4F00-A3DE-C961B96B9C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DD9AA1-75A2-48DE-9C43-63FDFA21329C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="-15" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,13 +59,6 @@
 5) Calculate the average  value of the "fartsgrens" field in the resulting sub-network. </t>
   </si>
   <si>
-    <t>Avg. speed: 64.8622047244094
-Dataset: "\\wsl.localhost\Ubuntu\home\dev\master-thesis\data\noisiest_roads_elveg.shp"</t>
-  </si>
-  <si>
-    <t>Dataset containing building points: "\\wsl.localhost\Ubuntu\home\dev\master-thesis\data\bygninger_100årsflom.shp"</t>
-  </si>
-  <si>
     <t>How many percent of buildings have more than 2km to the nearest "Videregående skole"?</t>
   </si>
   <si>
@@ -169,10 +162,6 @@
 3) Count the rows after filtering</t>
   </si>
   <si>
-    <t>Number of hotels: 28
-Dataset: "\\wsl.localhost\Ubuntu\home\dev\master-thesis\data\hotels.shp"</t>
-  </si>
-  <si>
     <t>Postal code</t>
   </si>
   <si>
@@ -184,6 +173,15 @@
 2) Find the "adresseTekst" attribute 
 3) Find the closest matching address, if any
 4) Get the entire row, and look up the "postnummer" attribute</t>
+  </si>
+  <si>
+    <t>Avg. speed: 64.8622047244094</t>
+  </si>
+  <si>
+    <t>Dataset containing building points</t>
+  </si>
+  <si>
+    <t>Number of hotels: 28</t>
   </si>
 </sst>
 </file>
@@ -546,139 +544,139 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="210" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C9" s="1">
         <v>7031</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>